<commit_message>
Updated report and release summary
</commit_message>
<xml_diff>
--- a/Iteration 2/Other/Agile Release Summary.xlsx
+++ b/Iteration 2/Other/Agile Release Summary.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>Conestoga College</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Transition</t>
   </si>
   <si>
-    <t>Due: Apr-24</t>
-  </si>
-  <si>
     <t>Feature / Requirement</t>
   </si>
   <si>
@@ -144,6 +141,9 @@
   </si>
   <si>
     <t>Due: Mar-8</t>
+  </si>
+  <si>
+    <t>Due:</t>
   </si>
 </sst>
 </file>
@@ -559,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,32 +574,34 @@
     <col min="6" max="6" width="14.140625" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="5" t="s">
         <v>4</v>
       </c>
@@ -607,55 +609,76 @@
         <v>4</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
         <v>27</v>
       </c>
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
       <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
         <v>27</v>
       </c>
-      <c r="F9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>101</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="8">
         <v>1</v>
@@ -664,12 +687,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>102</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="8">
         <v>1</v>
@@ -678,12 +701,12 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>103</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="8">
         <v>1.25</v>
@@ -692,12 +715,12 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>104</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="8">
         <v>1.25</v>
@@ -706,12 +729,12 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>105</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="8">
         <v>1.5</v>
@@ -720,12 +743,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>106</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="8">
         <v>1.5</v>
@@ -739,7 +762,7 @@
         <v>107</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="8">
         <v>1.5</v>
@@ -753,7 +776,7 @@
         <v>115</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="8">
         <v>1.25</v>
@@ -767,7 +790,7 @@
         <v>120</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="8">
         <v>3</v>
@@ -781,7 +804,7 @@
         <v>121</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="8">
         <v>1.5</v>
@@ -795,7 +818,7 @@
         <v>122</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="8">
         <v>1.5</v>
@@ -813,117 +836,133 @@
         <v>108</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
       <c r="E23" s="16">
         <v>4</v>
       </c>
-      <c r="F23" s="16"/>
+      <c r="F23" s="16">
+        <v>15</v>
+      </c>
     </row>
     <row r="24" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>109</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="E24" s="16">
         <v>4</v>
       </c>
-      <c r="F24" s="16"/>
+      <c r="F24" s="16">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>110</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="E25" s="16">
         <v>4.5</v>
       </c>
-      <c r="F25" s="16"/>
+      <c r="F25" s="16">
+        <v>5.75</v>
+      </c>
     </row>
     <row r="26" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>111</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
       <c r="E26" s="16">
         <v>4.5</v>
       </c>
-      <c r="F26" s="16"/>
+      <c r="F26" s="16">
+        <v>5.75</v>
+      </c>
     </row>
     <row r="27" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>112</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
       <c r="E27" s="16">
         <v>4</v>
       </c>
-      <c r="F27" s="16"/>
+      <c r="F27" s="16">
+        <v>2.25</v>
+      </c>
     </row>
     <row r="28" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>113</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
       <c r="E28" s="16">
         <v>3.5</v>
       </c>
-      <c r="F28" s="16"/>
+      <c r="F28" s="16">
+        <v>7.25</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>114</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C29" s="16"/>
       <c r="D29" s="16"/>
       <c r="E29" s="16">
         <v>3.5</v>
       </c>
-      <c r="F29" s="16"/>
+      <c r="F29" s="16">
+        <v>7.25</v>
+      </c>
     </row>
     <row r="30" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>116</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30" s="16"/>
       <c r="D30" s="16"/>
       <c r="E30" s="16">
         <v>1.5</v>
       </c>
-      <c r="F30" s="16"/>
+      <c r="F30" s="16">
+        <v>4.25</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -933,7 +972,7 @@
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -944,7 +983,7 @@
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C36" s="10">
         <f>SUM(C11:C21)</f>
@@ -960,7 +999,7 @@
       </c>
       <c r="F36" s="10">
         <f>SUM(F11:F35)</f>
-        <v>0</v>
+        <v>62.5</v>
       </c>
       <c r="G36" s="10">
         <f>SUM(G11:G35)</f>
@@ -968,33 +1007,33 @@
       </c>
       <c r="H36" s="11"/>
       <c r="I36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C38" s="10">
-        <f>SUM(C11:C21)</f>
-        <v>16.25</v>
+        <f>SUM(C36 + E36)</f>
+        <v>45.75</v>
       </c>
       <c r="I38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B39" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C39" s="10">
-        <f>SUM(D11:D21)</f>
-        <v>41.5</v>
+        <f>SUM(D36 + F36)</f>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>